<commit_message>
Added participant identifier scheme 0193
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v3.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v3.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$J$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$J$72</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="267">
   <si>
     <t>GLN</t>
   </si>
@@ -864,6 +864,20 @@
   </si>
   <si>
     <t>Temporary until ISO 6523 identifier approved</t>
+  </si>
+  <si>
+    <t>UBLPE</t>
+  </si>
+  <si>
+    <t>0193</t>
+  </si>
+  <si>
+    <t>UBL.BE</t>
+  </si>
+  <si>
+    <t>Maximum 50 characters
+4 Characters fixed length identifying the type 
+Maximum 46 characters for the identifier itself</t>
   </si>
 </sst>
 </file>
@@ -1373,11 +1387,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,25 +1792,25 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>3</v>
+        <v>263</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>264</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>4</v>
+        <v>265</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>106</v>
+        <v>261</v>
       </c>
       <c r="E17" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>80</v>
+        <v>266</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>67</v>
@@ -1804,13 +1818,13 @@
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>106</v>
@@ -1819,19 +1833,22 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>95</v>
+      <c r="G18" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>106</v>
@@ -1841,18 +1858,18 @@
         <v>0</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>106</v>
@@ -1865,15 +1882,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>106</v>
@@ -1883,18 +1900,18 @@
         <v>0</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>106</v>
@@ -1904,18 +1921,18 @@
         <v>0</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>106</v>
@@ -1924,13 +1941,16 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="I23" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>20</v>
@@ -1939,82 +1959,82 @@
         <v>106</v>
       </c>
       <c r="E24" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="I24" s="8">
+      <c r="F25" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="8">
         <v>990399123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E26" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>106</v>
@@ -2023,19 +2043,16 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="I28" s="8" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>106</v>
@@ -2044,94 +2061,94 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="I29" s="8" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E30" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E31" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="E32" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E32" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="E33" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>108</v>
@@ -2140,34 +2157,37 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="G34" s="8" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E35" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>174</v>
@@ -2179,13 +2199,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>174</v>
@@ -2197,13 +2217,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>174</v>
@@ -2215,13 +2235,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>174</v>
@@ -2233,13 +2253,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>174</v>
@@ -2251,13 +2271,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>174</v>
@@ -2269,13 +2289,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>174</v>
@@ -2287,13 +2307,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>174</v>
@@ -2305,13 +2325,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>174</v>
@@ -2323,31 +2343,31 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E45" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>174</v>
@@ -2359,13 +2379,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>120</v>
+        <v>207</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>174</v>
@@ -2377,13 +2397,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>174</v>
@@ -2395,13 +2415,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>174</v>
@@ -2413,13 +2433,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>174</v>
@@ -2431,13 +2451,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>210</v>
+        <v>157</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>174</v>
@@ -2449,13 +2469,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>158</v>
+        <v>210</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>174</v>
@@ -2467,13 +2487,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>174</v>
@@ -2485,13 +2505,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>174</v>
@@ -2503,49 +2523,49 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E55" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E55" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="D56" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E56" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E56" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>174</v>
@@ -2557,13 +2577,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>174</v>
@@ -2575,13 +2595,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>174</v>
@@ -2593,13 +2613,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>174</v>
@@ -2611,13 +2631,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>174</v>
@@ -2629,13 +2649,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>174</v>
@@ -2647,13 +2667,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>174</v>
@@ -2665,13 +2685,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>174</v>
@@ -2683,13 +2703,13 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>174</v>
@@ -2701,112 +2721,109 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E66" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E66" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+      <c r="D67" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E67" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E67" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="D68" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E68" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E68" s="6" t="b">
+      <c r="E69" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E69" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E70" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>230</v>
@@ -2815,30 +2832,51 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="G71" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E72" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E72" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="J72" s="2" t="s">
+      <c r="E73" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J73" s="2" t="s">
         <v>262</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J71"/>
+  <autoFilter ref="A1:J72"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>